<commit_message>
Initial Commit Estimation tool
</commit_message>
<xml_diff>
--- a/Estimation_NC/media/Estimation.xlsx
+++ b/Estimation_NC/media/Estimation.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Estimation_Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Estimation_LL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Simple</t>
   </si>
@@ -45,12 +46,36 @@
   </si>
   <si>
     <t>Final_Tech_LOE</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple </t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Trans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,13 +128,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +422,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,4 +660,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated UI for Estimation for HL and LL
</commit_message>
<xml_diff>
--- a/Estimation_NC/media/Estimation.xlsx
+++ b/Estimation_NC/media/Estimation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation_Matrix" sheetId="1" r:id="rId1"/>
@@ -54,28 +54,25 @@
     <t>Weights</t>
   </si>
   <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Trans</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simple </t>
-  </si>
-  <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>UT</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Trans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,19 +661,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -684,80 +680,80 @@
         <v>8</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
         <v>10</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="6">
         <v>0.5</v>
       </c>
-      <c r="E2" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="F2" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C4" s="6">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D4" s="6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
       </c>
       <c r="F4" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M6" s="7"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final Commit for the estimation Tool
</commit_message>
<xml_diff>
--- a/Estimation_NC/media/Estimation.xlsx
+++ b/Estimation_NC/media/Estimation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>Simple</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Trans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simple </t>
   </si>
 </sst>
 </file>
@@ -664,7 +661,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +691,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>

</xml_diff>